<commit_message>
Final results5 and new Assignment6
</commit_message>
<xml_diff>
--- a/Total results.xlsx
+++ b/Total results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="19">
   <si>
     <t>Асеев</t>
   </si>
@@ -43,16 +43,34 @@
     <t>Сорокин</t>
   </si>
   <si>
-    <t>Петоров</t>
-  </si>
-  <si>
     <t>н</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
-    <t>Средний балл</t>
+    <t>5-</t>
+  </si>
+  <si>
+    <t>4-</t>
+  </si>
+  <si>
+    <t>Петров</t>
+  </si>
+  <si>
+    <t>3-</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>отсутствие</t>
+  </si>
+  <si>
+    <t>предложил темы проекта</t>
+  </si>
+  <si>
+    <t>ничего не предложил</t>
   </si>
 </sst>
 </file>
@@ -88,7 +106,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -99,6 +117,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -404,21 +431,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S23"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="10.140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
+      <c r="A1" s="6"/>
       <c r="B1" s="3">
         <v>42254</v>
       </c>
@@ -431,7 +458,9 @@
       <c r="E1" s="3">
         <v>42275</v>
       </c>
-      <c r="F1" s="1"/>
+      <c r="F1" s="3">
+        <v>42282</v>
+      </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -447,16 +476,20 @@
       <c r="S1" s="1"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
-      <c r="E2" s="4">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1"/>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -472,16 +505,20 @@
       <c r="S2" s="1"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="4">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1"/>
+      <c r="E3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -497,18 +534,22 @@
       <c r="S3" s="1"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="4">
-        <v>9</v>
-      </c>
-      <c r="F4" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -524,18 +565,20 @@
       <c r="S4" s="1"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4">
-        <v>7</v>
-      </c>
-      <c r="F5" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -551,20 +594,24 @@
       <c r="S5" s="1"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="C6" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" s="4">
         <v>0</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="2">
+        <v>2</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -580,16 +627,20 @@
       <c r="S6" s="1"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4">
-        <v>7</v>
-      </c>
-      <c r="F7" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="F7" s="2">
+        <v>4</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -605,16 +656,20 @@
       <c r="S7" s="1"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="4">
-        <v>8</v>
-      </c>
-      <c r="F8" s="1"/>
+      <c r="E8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -630,20 +685,24 @@
       <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="4">
-        <v>7</v>
-      </c>
-      <c r="F9" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="2">
+        <v>3</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -659,16 +718,20 @@
       <c r="S9" s="1"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4">
-        <v>8</v>
-      </c>
-      <c r="F10" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -684,18 +747,22 @@
       <c r="S10" s="1"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -711,97 +778,27 @@
       <c r="S11" s="1"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>12</v>
+      <c r="A13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="2">
-        <f>AVERAGE(B2:T2)</f>
-        <v>8</v>
+      <c r="A14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="2">
-        <f>AVERAGE(B3:T3)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="2">
-        <f>AVERAGE(B4:T4)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="2">
-        <f>AVERAGE(B5:T5)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="2">
-        <f>AVERAGE(B6:T6)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="2">
-        <f>AVERAGE(B7:T7)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="2">
-        <f>AVERAGE(B8:T8)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="2">
-        <f>AVERAGE(B9:T9)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="2">
-        <f>AVERAGE(B10:T10)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>11</v>
+      <c r="A15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1st turn passed, 2nd begins
</commit_message>
<xml_diff>
--- a/Total results.xlsx
+++ b/Total results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="23">
   <si>
     <t>Асеев</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>2+</t>
+  </si>
+  <si>
+    <t>16.11.15.</t>
   </si>
 </sst>
 </file>
@@ -444,7 +447,7 @@
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,6 +458,7 @@
     <col min="7" max="9" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -489,7 +493,9 @@
       <c r="K1" s="8">
         <v>42317</v>
       </c>
-      <c r="L1" s="1"/>
+      <c r="L1" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -528,7 +534,9 @@
       <c r="K2" s="2">
         <v>5</v>
       </c>
-      <c r="L2" s="1"/>
+      <c r="L2" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -567,7 +575,9 @@
       <c r="K3" s="2">
         <v>5</v>
       </c>
-      <c r="L3" s="1"/>
+      <c r="L3" s="4">
+        <v>5</v>
+      </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
@@ -608,7 +618,9 @@
       <c r="K4" s="2">
         <v>5</v>
       </c>
-      <c r="L4" s="1"/>
+      <c r="L4" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -647,7 +659,9 @@
       <c r="K5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="1"/>
+      <c r="L5" s="4">
+        <v>4</v>
+      </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -690,7 +704,9 @@
       <c r="K6" s="2">
         <v>3</v>
       </c>
-      <c r="L6" s="1"/>
+      <c r="L6" s="4">
+        <v>4</v>
+      </c>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -729,7 +745,9 @@
       <c r="K7" s="2">
         <v>2</v>
       </c>
-      <c r="L7" s="1"/>
+      <c r="L7" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -768,7 +786,9 @@
       <c r="K8" s="2">
         <v>5</v>
       </c>
-      <c r="L8" s="1"/>
+      <c r="L8" s="4">
+        <v>5</v>
+      </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
@@ -811,7 +831,9 @@
       <c r="K9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L9" s="1"/>
+      <c r="L9" s="4">
+        <v>5</v>
+      </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
@@ -850,7 +872,9 @@
       <c r="K10" s="2">
         <v>5</v>
       </c>
-      <c r="L10" s="1"/>
+      <c r="L10" s="4">
+        <v>5</v>
+      </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
@@ -891,7 +915,9 @@
       <c r="K11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L11" s="1"/>
+      <c r="L11" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>

</xml_diff>

<commit_message>
end of 14 week
</commit_message>
<xml_diff>
--- a/Total results.xlsx
+++ b/Total results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="23">
   <si>
     <t>Асеев</t>
   </si>
@@ -447,7 +447,7 @@
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,6 +460,7 @@
     <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.140625" style="2"/>
     <col min="13" max="14" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -503,7 +504,9 @@
       <c r="N1" s="8">
         <v>42338</v>
       </c>
-      <c r="O1" s="1"/>
+      <c r="O1" s="3">
+        <v>42345</v>
+      </c>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
@@ -548,7 +551,9 @@
       <c r="N2" s="2">
         <v>5</v>
       </c>
-      <c r="O2" s="1"/>
+      <c r="O2" s="4">
+        <v>5</v>
+      </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
@@ -593,7 +598,9 @@
       <c r="N3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="1"/>
+      <c r="O3" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
@@ -640,7 +647,9 @@
       <c r="N4" s="2">
         <v>5</v>
       </c>
-      <c r="O4" s="1"/>
+      <c r="O4" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
@@ -685,7 +694,9 @@
       <c r="N5" s="2">
         <v>4</v>
       </c>
-      <c r="O5" s="1"/>
+      <c r="O5" s="4">
+        <v>4</v>
+      </c>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
@@ -734,7 +745,9 @@
       <c r="N6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O6" s="1"/>
+      <c r="O6" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
@@ -779,7 +792,9 @@
       <c r="N7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O7" s="1"/>
+      <c r="O7" s="4">
+        <v>5</v>
+      </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
@@ -824,7 +839,9 @@
       <c r="N8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O8" s="1"/>
+      <c r="O8" s="4">
+        <v>5</v>
+      </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
@@ -873,7 +890,9 @@
       <c r="N9" s="2">
         <v>5</v>
       </c>
-      <c r="O9" s="1"/>
+      <c r="O9" s="4">
+        <v>5</v>
+      </c>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
@@ -918,7 +937,9 @@
       <c r="N10" s="2">
         <v>5</v>
       </c>
-      <c r="O10" s="1"/>
+      <c r="O10" s="4">
+        <v>5</v>
+      </c>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
@@ -965,7 +986,7 @@
       <c r="N11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="O11" s="1"/>
+      <c r="O11" s="4"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>

</xml_diff>

<commit_message>
end of 15th week
</commit_message>
<xml_diff>
--- a/Total results.xlsx
+++ b/Total results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="23">
   <si>
     <t>Асеев</t>
   </si>
@@ -447,7 +447,7 @@
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,7 +460,7 @@
     <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.140625" style="2"/>
     <col min="13" max="14" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -507,7 +507,9 @@
       <c r="O1" s="3">
         <v>42345</v>
       </c>
-      <c r="P1" s="1"/>
+      <c r="P1" s="3">
+        <v>42352</v>
+      </c>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
@@ -554,7 +556,9 @@
       <c r="O2" s="4">
         <v>5</v>
       </c>
-      <c r="P2" s="1"/>
+      <c r="P2" s="4">
+        <v>5</v>
+      </c>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
@@ -601,7 +605,9 @@
       <c r="O3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="1"/>
+      <c r="P3" s="4">
+        <v>5</v>
+      </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
@@ -650,7 +656,9 @@
       <c r="O4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="P4" s="1"/>
+      <c r="P4" s="4">
+        <v>5</v>
+      </c>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
@@ -697,7 +705,9 @@
       <c r="O5" s="4">
         <v>4</v>
       </c>
-      <c r="P5" s="1"/>
+      <c r="P5" s="4">
+        <v>5</v>
+      </c>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
@@ -748,7 +758,9 @@
       <c r="O6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="P6" s="1"/>
+      <c r="P6" s="4">
+        <v>2</v>
+      </c>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
@@ -795,7 +807,9 @@
       <c r="O7" s="4">
         <v>5</v>
       </c>
-      <c r="P7" s="1"/>
+      <c r="P7" s="4">
+        <v>5</v>
+      </c>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
@@ -842,7 +856,9 @@
       <c r="O8" s="4">
         <v>5</v>
       </c>
-      <c r="P8" s="1"/>
+      <c r="P8" s="4">
+        <v>5</v>
+      </c>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
@@ -893,7 +909,9 @@
       <c r="O9" s="4">
         <v>5</v>
       </c>
-      <c r="P9" s="1"/>
+      <c r="P9" s="4">
+        <v>5</v>
+      </c>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
@@ -940,7 +958,9 @@
       <c r="O10" s="4">
         <v>5</v>
       </c>
-      <c r="P10" s="1"/>
+      <c r="P10" s="4">
+        <v>5</v>
+      </c>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
@@ -986,8 +1006,12 @@
       <c r="N11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="O11" s="4"/>
-      <c r="P11" s="1"/>
+      <c r="O11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>

</xml_diff>